<commit_message>
SD: started classifying SD DENR terms
</commit_message>
<xml_diff>
--- a/Vocabularies/SD/sd-denr-d.xlsx
+++ b/Vocabularies/SD/sd-denr-d.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph/Desktop/WSWC/IoW/Vocabularies/SD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E570B902-6CC8-B748-9845-FADAFE573DC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ED18B8-6F5E-2C49-85BB-56E405BFE81D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36260" yWindow="1480" windowWidth="32280" windowHeight="16760" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
@@ -611,12 +611,6 @@
   </si>
   <si>
     <t>Well screen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-To give up the right to make a beneficial use of water as authorized by a water_x000D_
-        appropriation  SDCL 46-5-37.1.
-</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1825,6 +1819,10 @@
 Water Rights  Well Construction Standards: ARSD 74:02:04:20 The intake_x000D_
         structure of a well which allows water to enter the well and which helps prevent formation_x000D_
         material from entering with the water.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To give up the right to make a beneficial use of water as authorized by a water appropriation  SDCL 46-5-37.1.
 </t>
   </si>
 </sst>
@@ -1866,12 +1864,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2188,15 +2189,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E542F74-ACD9-49CD-B312-AB6D05B8D550}">
   <dimension ref="A1:I163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="34.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="255.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -2228,12 +2229,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>195</v>
+      <c r="C2" s="3" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2241,7 +2242,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2249,7 +2250,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2257,7 +2258,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -2265,7 +2266,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2273,7 +2274,7 @@
         <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -2281,7 +2282,7 @@
         <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -2289,7 +2290,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2297,7 +2298,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -2305,7 +2306,7 @@
         <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -2313,7 +2314,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -2321,7 +2322,7 @@
         <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2329,7 +2330,7 @@
         <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2337,7 +2338,7 @@
         <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -2345,7 +2346,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2353,7 +2354,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2361,7 +2362,7 @@
         <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2369,7 +2370,7 @@
         <v>50</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2377,7 +2378,7 @@
         <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2385,7 +2386,7 @@
         <v>52</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2393,7 +2394,7 @@
         <v>53</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2401,7 +2402,7 @@
         <v>54</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2409,7 +2410,7 @@
         <v>55</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2417,7 +2418,7 @@
         <v>56</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2425,7 +2426,7 @@
         <v>57</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2433,7 +2434,7 @@
         <v>58</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2441,7 +2442,7 @@
         <v>59</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2449,7 +2450,7 @@
         <v>60</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2457,7 +2458,7 @@
         <v>61</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2465,7 +2466,7 @@
         <v>62</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2473,7 +2474,7 @@
         <v>63</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2481,7 +2482,7 @@
         <v>64</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2489,7 +2490,7 @@
         <v>65</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2497,7 +2498,7 @@
         <v>66</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2505,7 +2506,7 @@
         <v>67</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2513,7 +2514,7 @@
         <v>68</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2521,7 +2522,7 @@
         <v>69</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2529,7 +2530,7 @@
         <v>70</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2537,7 +2538,7 @@
         <v>71</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2545,7 +2546,7 @@
         <v>72</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2553,7 +2554,7 @@
         <v>73</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2561,7 +2562,7 @@
         <v>74</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2569,7 +2570,7 @@
         <v>75</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2577,7 +2578,7 @@
         <v>76</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2585,7 +2586,7 @@
         <v>77</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2593,7 +2594,7 @@
         <v>78</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -2601,7 +2602,7 @@
         <v>79</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2609,7 +2610,7 @@
         <v>80</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2617,7 +2618,7 @@
         <v>81</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2625,7 +2626,7 @@
         <v>82</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2633,7 +2634,7 @@
         <v>83</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2641,7 +2642,7 @@
         <v>84</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2649,7 +2650,7 @@
         <v>85</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2657,7 +2658,7 @@
         <v>86</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2665,7 +2666,7 @@
         <v>87</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2673,7 +2674,7 @@
         <v>88</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2681,7 +2682,7 @@
         <v>89</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2689,7 +2690,7 @@
         <v>90</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2697,7 +2698,7 @@
         <v>91</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2705,7 +2706,7 @@
         <v>92</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -2713,7 +2714,7 @@
         <v>93</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -2721,7 +2722,7 @@
         <v>94</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -2729,7 +2730,7 @@
         <v>95</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2737,7 +2738,7 @@
         <v>96</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2745,7 +2746,7 @@
         <v>97</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2753,7 +2754,7 @@
         <v>98</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2761,7 +2762,7 @@
         <v>99</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -2769,7 +2770,7 @@
         <v>100</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2777,7 +2778,7 @@
         <v>101</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2785,7 +2786,7 @@
         <v>102</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -2793,7 +2794,7 @@
         <v>103</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2801,7 +2802,7 @@
         <v>104</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2809,7 +2810,7 @@
         <v>105</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2817,7 +2818,7 @@
         <v>106</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2825,7 +2826,7 @@
         <v>107</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2833,7 +2834,7 @@
         <v>108</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -2841,7 +2842,7 @@
         <v>109</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -2849,7 +2850,7 @@
         <v>110</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2857,7 +2858,7 @@
         <v>111</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2865,7 +2866,7 @@
         <v>112</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -2873,7 +2874,7 @@
         <v>113</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2881,7 +2882,7 @@
         <v>114</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2889,7 +2890,7 @@
         <v>115</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2897,7 +2898,7 @@
         <v>116</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2905,7 +2906,7 @@
         <v>117</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -2913,7 +2914,7 @@
         <v>118</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -2921,7 +2922,7 @@
         <v>119</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2929,7 +2930,7 @@
         <v>120</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -2937,7 +2938,7 @@
         <v>121</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -2945,7 +2946,7 @@
         <v>122</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -2953,7 +2954,7 @@
         <v>123</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -2961,7 +2962,7 @@
         <v>124</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2969,7 +2970,7 @@
         <v>125</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2977,7 +2978,7 @@
         <v>126</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -2985,7 +2986,7 @@
         <v>127</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2993,7 +2994,7 @@
         <v>128</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -3001,7 +3002,7 @@
         <v>129</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -3009,7 +3010,7 @@
         <v>130</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -3017,7 +3018,7 @@
         <v>131</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -3025,7 +3026,7 @@
         <v>132</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -3033,7 +3034,7 @@
         <v>133</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -3041,7 +3042,7 @@
         <v>134</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -3049,7 +3050,7 @@
         <v>135</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -3057,7 +3058,7 @@
         <v>136</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -3065,7 +3066,7 @@
         <v>137</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -3073,7 +3074,7 @@
         <v>138</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -3081,7 +3082,7 @@
         <v>139</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -3089,7 +3090,7 @@
         <v>140</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -3097,7 +3098,7 @@
         <v>141</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -3105,7 +3106,7 @@
         <v>142</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -3113,7 +3114,7 @@
         <v>143</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -3121,7 +3122,7 @@
         <v>144</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -3129,7 +3130,7 @@
         <v>145</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -3137,7 +3138,7 @@
         <v>146</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -3145,7 +3146,7 @@
         <v>147</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -3153,7 +3154,7 @@
         <v>148</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -3161,7 +3162,7 @@
         <v>149</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -3169,7 +3170,7 @@
         <v>150</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -3177,7 +3178,7 @@
         <v>151</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -3185,7 +3186,7 @@
         <v>152</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -3193,7 +3194,7 @@
         <v>153</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -3201,7 +3202,7 @@
         <v>154</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -3209,7 +3210,7 @@
         <v>155</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -3217,7 +3218,7 @@
         <v>156</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -3225,7 +3226,7 @@
         <v>157</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -3233,7 +3234,7 @@
         <v>158</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -3241,7 +3242,7 @@
         <v>159</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -3249,7 +3250,7 @@
         <v>160</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -3257,7 +3258,7 @@
         <v>161</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -3265,7 +3266,7 @@
         <v>162</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -3273,7 +3274,7 @@
         <v>163</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -3281,7 +3282,7 @@
         <v>164</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -3289,7 +3290,7 @@
         <v>165</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -3297,7 +3298,7 @@
         <v>166</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -3305,7 +3306,7 @@
         <v>167</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -3313,7 +3314,7 @@
         <v>168</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -3321,7 +3322,7 @@
         <v>169</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -3329,7 +3330,7 @@
         <v>170</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -3337,7 +3338,7 @@
         <v>171</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
@@ -3345,7 +3346,7 @@
         <v>172</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -3353,7 +3354,7 @@
         <v>173</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
@@ -3361,7 +3362,7 @@
         <v>174</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -3369,7 +3370,7 @@
         <v>175</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
@@ -3377,7 +3378,7 @@
         <v>176</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
@@ -3385,7 +3386,7 @@
         <v>177</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -3393,7 +3394,7 @@
         <v>178</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
@@ -3401,7 +3402,7 @@
         <v>179</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
@@ -3409,7 +3410,7 @@
         <v>180</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
@@ -3417,7 +3418,7 @@
         <v>181</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
@@ -3425,7 +3426,7 @@
         <v>182</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -3433,7 +3434,7 @@
         <v>183</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
@@ -3441,7 +3442,7 @@
         <v>184</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
@@ -3449,7 +3450,7 @@
         <v>185</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
@@ -3457,7 +3458,7 @@
         <v>186</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -3465,7 +3466,7 @@
         <v>187</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
@@ -3473,7 +3474,7 @@
         <v>188</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
@@ -3481,7 +3482,7 @@
         <v>189</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
@@ -3489,7 +3490,7 @@
         <v>190</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
@@ -3497,7 +3498,7 @@
         <v>191</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
@@ -3505,7 +3506,7 @@
         <v>192</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -3513,7 +3514,7 @@
         <v>193</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
@@ -3521,7 +3522,7 @@
         <v>194</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update TX and SD xlsx to include themes and vocab metadata
</commit_message>
<xml_diff>
--- a/Vocabularies/SD/sd-denr-d.xlsx
+++ b/Vocabularies/SD/sd-denr-d.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph/Desktop/WSWC/IoW/Vocabularies/SD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kso8/Box/Internet Of Water/GitHub/Glossary/Vocabularies/SD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9FE4EA-52A2-AA4B-A9A0-1BBD2DBCF4CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C44241-B4A8-DC46-A9FE-7C509EA3F730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
+    <workbookView xWindow="5180" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="361">
   <si>
     <t>Term</t>
   </si>
@@ -1098,6 +1098,21 @@
   </si>
   <si>
     <t>Water Rights  Well Construction Standards: ARSD 74:02:04:20 The intake structure of a well which allows water to enter the well and which helps prevent formation material from entering with the water.</t>
+  </si>
+  <si>
+    <t>South Dakota Department of Environment &amp; Natural Resources</t>
+  </si>
+  <si>
+    <t>SD-DENR</t>
+  </si>
+  <si>
+    <t>SD-DENR Dictionary of Water Right Terms</t>
+  </si>
+  <si>
+    <t>sd-denr-dwrt</t>
+  </si>
+  <si>
+    <t>https://denr.sd.gov/des/wr/dictionary.aspx</t>
   </si>
 </sst>
 </file>
@@ -1481,7 +1496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E542F74-ACD9-49CD-B312-AB6D05B8D550}">
   <dimension ref="A1:I163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A134" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
@@ -3475,8 +3490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251B0935-F8C3-480F-B897-E642A4205A23}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3517,6 +3532,21 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D2" t="s">
+        <v>359</v>
+      </c>
+      <c r="F2" t="s">
+        <v>360</v>
+      </c>
       <c r="G2" t="s">
         <v>26</v>
       </c>

</xml_diff>